<commit_message>
Updated permissions for document repository.
</commit_message>
<xml_diff>
--- a/Roles and Permissions.xlsx
+++ b/Roles and Permissions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tayyab.asghar\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\permissions\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="ScreenIds" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Z_49968090_594F_4035_ABCC_088176AC5527_.wvu.FilterData" localSheetId="0" hidden="1">'Roles and Permissions'!$A$1:$A$955</definedName>
+    <definedName name="Z_49968090_594F_4035_ABCC_088176AC5527_.wvu.FilterData" localSheetId="0" hidden="1">'Roles and Permissions'!$A$1:$A$958</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <customWorkbookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="91">
   <si>
     <t>User</t>
   </si>
@@ -309,6 +309,9 @@
   </si>
   <si>
     <t>customer-admin-comp</t>
+  </si>
+  <si>
+    <t>document-repository-comp</t>
   </si>
 </sst>
 </file>
@@ -697,10 +700,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Y955"/>
+  <dimension ref="A1:Y958"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C156" sqref="C156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1538,14 +1541,14 @@
       <c r="B22" s="2">
         <v>21</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>10</v>
@@ -1581,10 +1584,10 @@
         <v>7</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>10</v>
@@ -1620,7 +1623,7 @@
         <v>11</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>30</v>
@@ -1659,13 +1662,13 @@
         <v>11</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
@@ -1698,13 +1701,13 @@
         <v>11</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -1734,13 +1737,13 @@
         <v>26</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>10</v>
@@ -1772,14 +1775,14 @@
       <c r="B28" s="2">
         <v>27</v>
       </c>
-      <c r="C28" s="5" t="s">
-        <v>11</v>
+      <c r="C28" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>10</v>
@@ -1815,7 +1818,7 @@
         <v>11</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>35</v>
@@ -1854,7 +1857,7 @@
         <v>11</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>35</v>
@@ -1893,13 +1896,13 @@
         <v>11</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>35</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
@@ -1932,13 +1935,13 @@
         <v>11</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
@@ -1961,82 +1964,82 @@
       <c r="Y32" s="2"/>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>42</v>
+      <c r="A33" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="B33" s="2">
         <v>32</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>7</v>
+      <c r="C33" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F33" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F33" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
-      <c r="M33" s="3"/>
-      <c r="N33" s="3"/>
-      <c r="O33" s="3"/>
-      <c r="P33" s="3"/>
-      <c r="Q33" s="3"/>
-      <c r="R33" s="3"/>
-      <c r="S33" s="3"/>
-      <c r="T33" s="3"/>
-      <c r="U33" s="3"/>
-      <c r="V33" s="3"/>
-      <c r="W33" s="3"/>
-      <c r="X33" s="3"/>
-      <c r="Y33" s="3"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
+      <c r="R33" s="2"/>
+      <c r="S33" s="2"/>
+      <c r="T33" s="2"/>
+      <c r="U33" s="2"/>
+      <c r="V33" s="2"/>
+      <c r="W33" s="2"/>
+      <c r="X33" s="2"/>
+      <c r="Y33" s="2"/>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B34" s="2">
         <v>33</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E34" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E34" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F34" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
-      <c r="M34" s="2"/>
-      <c r="N34" s="2"/>
-      <c r="O34" s="2"/>
-      <c r="P34" s="2"/>
-      <c r="Q34" s="2"/>
-      <c r="R34" s="2"/>
-      <c r="S34" s="2"/>
-      <c r="T34" s="2"/>
-      <c r="U34" s="2"/>
-      <c r="V34" s="2"/>
-      <c r="W34" s="2"/>
-      <c r="X34" s="2"/>
-      <c r="Y34" s="2"/>
+      <c r="F34" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3"/>
+      <c r="P34" s="3"/>
+      <c r="Q34" s="3"/>
+      <c r="R34" s="3"/>
+      <c r="S34" s="3"/>
+      <c r="T34" s="3"/>
+      <c r="U34" s="3"/>
+      <c r="V34" s="3"/>
+      <c r="W34" s="3"/>
+      <c r="X34" s="3"/>
+      <c r="Y34" s="3"/>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
@@ -2049,13 +2052,13 @@
         <v>7</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
@@ -2088,7 +2091,7 @@
         <v>7</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>9</v>
@@ -2124,16 +2127,16 @@
         <v>36</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
@@ -2166,7 +2169,7 @@
         <v>11</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>88</v>
+        <v>18</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>17</v>
@@ -2205,7 +2208,7 @@
         <v>11</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>20</v>
+        <v>88</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>17</v>
@@ -2244,7 +2247,7 @@
         <v>11</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>17</v>
@@ -2279,11 +2282,11 @@
       <c r="B41" s="2">
         <v>40</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>17</v>
@@ -2322,7 +2325,7 @@
         <v>11</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>17</v>
@@ -2357,11 +2360,11 @@
       <c r="B43" s="2">
         <v>42</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C43" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>17</v>
@@ -2391,22 +2394,22 @@
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B44" s="2">
         <v>43</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
@@ -2436,13 +2439,13 @@
         <v>44</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>10</v>
@@ -2478,10 +2481,10 @@
         <v>11</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E46" s="15" t="s">
         <v>13</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>10</v>
@@ -2516,8 +2519,8 @@
       <c r="C47" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D47" s="10" t="s">
-        <v>14</v>
+      <c r="D47" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="E47" s="15" t="s">
         <v>13</v>
@@ -2546,7 +2549,7 @@
       <c r="Y47" s="2"/>
     </row>
     <row r="48" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A48" s="15" t="s">
+      <c r="A48" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B48" s="2">
@@ -2556,10 +2559,10 @@
         <v>11</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>78</v>
+        <v>14</v>
       </c>
       <c r="E48" s="15" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>10</v>
@@ -2585,7 +2588,7 @@
       <c r="Y48" s="2"/>
     </row>
     <row r="49" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="15" t="s">
         <v>44</v>
       </c>
       <c r="B49" s="2">
@@ -2594,8 +2597,8 @@
       <c r="C49" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D49" s="3" t="s">
-        <v>15</v>
+      <c r="D49" s="10" t="s">
+        <v>78</v>
       </c>
       <c r="E49" s="15" t="s">
         <v>8</v>
@@ -2634,9 +2637,9 @@
         <v>11</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E50" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E50" s="15" t="s">
         <v>8</v>
       </c>
       <c r="F50" s="2" t="s">
@@ -2670,16 +2673,16 @@
         <v>50</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
@@ -2709,13 +2712,13 @@
         <v>51</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>19</v>
@@ -2751,7 +2754,7 @@
         <v>11</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>88</v>
+        <v>18</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>17</v>
@@ -2790,7 +2793,7 @@
         <v>11</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>20</v>
+        <v>88</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>17</v>
@@ -2829,7 +2832,7 @@
         <v>11</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>17</v>
@@ -2868,7 +2871,7 @@
         <v>11</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>17</v>
@@ -2907,7 +2910,7 @@
         <v>11</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>17</v>
@@ -2946,7 +2949,7 @@
         <v>11</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>17</v>
@@ -2982,16 +2985,16 @@
         <v>58</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
@@ -3024,7 +3027,7 @@
         <v>7</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>9</v>
@@ -3060,16 +3063,16 @@
         <v>60</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
@@ -3098,11 +3101,11 @@
       <c r="B62" s="2">
         <v>61</v>
       </c>
-      <c r="C62" s="5" t="s">
+      <c r="C62" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>26</v>
@@ -3141,7 +3144,7 @@
         <v>11</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>26</v>
@@ -3176,17 +3179,17 @@
       <c r="B64" s="2">
         <v>63</v>
       </c>
-      <c r="C64" s="2" t="s">
-        <v>7</v>
+      <c r="C64" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
@@ -3219,10 +3222,10 @@
         <v>7</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F65" s="2" t="s">
         <v>10</v>
@@ -3255,13 +3258,13 @@
         <v>65</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>32</v>
+        <v>7</v>
+      </c>
+      <c r="D66" s="10" t="s">
+        <v>90</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="F66" s="2" t="s">
         <v>10</v>
@@ -3297,13 +3300,13 @@
         <v>11</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
@@ -3336,7 +3339,7 @@
         <v>11</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>30</v>
@@ -3372,13 +3375,13 @@
         <v>68</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>19</v>
@@ -3410,17 +3413,17 @@
       <c r="B70" s="2">
         <v>69</v>
       </c>
-      <c r="C70" s="5" t="s">
+      <c r="C70" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
@@ -3449,14 +3452,14 @@
       <c r="B71" s="2">
         <v>70</v>
       </c>
-      <c r="C71" s="5" t="s">
-        <v>11</v>
+      <c r="C71" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>19</v>
@@ -3492,7 +3495,7 @@
         <v>11</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>45</v>
@@ -3528,13 +3531,13 @@
         <v>72</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="F73" s="2" t="s">
         <v>19</v>
@@ -3570,13 +3573,13 @@
         <v>11</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
@@ -3600,22 +3603,22 @@
     </row>
     <row r="75" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B75" s="2">
         <v>74</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="C75" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
@@ -3639,22 +3642,22 @@
     </row>
     <row r="76" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B76" s="2">
         <v>75</v>
       </c>
-      <c r="C76" s="2" t="s">
-        <v>7</v>
+      <c r="C76" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
@@ -3684,16 +3687,16 @@
         <v>76</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
@@ -3723,13 +3726,13 @@
         <v>77</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>88</v>
+        <v>17</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F78" s="2" t="s">
         <v>19</v>
@@ -3765,7 +3768,7 @@
         <v>11</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>17</v>
@@ -3804,7 +3807,7 @@
         <v>11</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>21</v>
+        <v>88</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>17</v>
@@ -3843,7 +3846,7 @@
         <v>11</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>17</v>
@@ -3882,7 +3885,7 @@
         <v>11</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>17</v>
@@ -3921,7 +3924,7 @@
         <v>11</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>17</v>
@@ -3957,13 +3960,13 @@
         <v>83</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F84" s="2" t="s">
         <v>19</v>
@@ -3999,10 +4002,10 @@
         <v>11</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="F85" s="2" t="s">
         <v>19</v>
@@ -4035,13 +4038,13 @@
         <v>85</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="F86" s="2" t="s">
         <v>19</v>
@@ -4077,7 +4080,7 @@
         <v>11</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>51</v>
@@ -4112,11 +4115,11 @@
       <c r="B88" s="2">
         <v>87</v>
       </c>
-      <c r="C88" s="5" t="s">
+      <c r="C88" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>51</v>
@@ -4151,11 +4154,11 @@
       <c r="B89" s="2">
         <v>88</v>
       </c>
-      <c r="C89" s="5" t="s">
+      <c r="C89" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>51</v>
@@ -4190,17 +4193,17 @@
       <c r="B90" s="2">
         <v>89</v>
       </c>
-      <c r="C90" s="2" t="s">
-        <v>7</v>
+      <c r="C90" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
@@ -4229,17 +4232,17 @@
       <c r="B91" s="2">
         <v>90</v>
       </c>
-      <c r="C91" s="2" t="s">
-        <v>7</v>
+      <c r="C91" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
@@ -4268,17 +4271,17 @@
       <c r="B92" s="2">
         <v>91</v>
       </c>
-      <c r="C92" s="5" t="s">
-        <v>11</v>
+      <c r="C92" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
@@ -4307,17 +4310,17 @@
       <c r="B93" s="2">
         <v>92</v>
       </c>
-      <c r="C93" s="5" t="s">
-        <v>11</v>
+      <c r="C93" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
@@ -4350,7 +4353,7 @@
         <v>11</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>26</v>
@@ -4386,16 +4389,16 @@
         <v>94</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
@@ -4428,13 +4431,13 @@
         <v>11</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
@@ -4464,13 +4467,13 @@
         <v>96</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="F97" s="2" t="s">
         <v>10</v>
@@ -4506,13 +4509,13 @@
         <v>11</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
@@ -4545,13 +4548,13 @@
         <v>11</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
@@ -4584,13 +4587,13 @@
         <v>11</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G100" s="2"/>
       <c r="H100" s="2"/>
@@ -4623,7 +4626,7 @@
         <v>11</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>57</v>
@@ -4662,13 +4665,13 @@
         <v>11</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G102" s="2"/>
       <c r="H102" s="2"/>
@@ -4701,13 +4704,13 @@
         <v>11</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G103" s="2"/>
       <c r="H103" s="2"/>
@@ -4740,13 +4743,13 @@
         <v>11</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E104" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G104" s="2"/>
       <c r="H104" s="2"/>
@@ -4768,44 +4771,44 @@
       <c r="X104" s="2"/>
       <c r="Y104" s="2"/>
     </row>
-    <row r="105" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="13" t="s">
+    <row r="105" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B105" s="2">
         <v>104</v>
       </c>
-      <c r="C105" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D105" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="E105" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F105" s="13" t="s">
+      <c r="C105" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F105" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G105" s="13"/>
-      <c r="H105" s="13"/>
-      <c r="I105" s="13"/>
-      <c r="J105" s="13"/>
-      <c r="K105" s="13"/>
-      <c r="L105" s="13"/>
-      <c r="M105" s="13"/>
-      <c r="N105" s="13"/>
-      <c r="O105" s="13"/>
-      <c r="P105" s="13"/>
-      <c r="Q105" s="13"/>
-      <c r="R105" s="13"/>
-      <c r="S105" s="13"/>
-      <c r="T105" s="13"/>
-      <c r="U105" s="13"/>
-      <c r="V105" s="13"/>
-      <c r="W105" s="13"/>
-      <c r="X105" s="13"/>
-      <c r="Y105" s="13"/>
+      <c r="G105" s="2"/>
+      <c r="H105" s="2"/>
+      <c r="I105" s="2"/>
+      <c r="J105" s="2"/>
+      <c r="K105" s="2"/>
+      <c r="L105" s="2"/>
+      <c r="M105" s="2"/>
+      <c r="N105" s="2"/>
+      <c r="O105" s="2"/>
+      <c r="P105" s="2"/>
+      <c r="Q105" s="2"/>
+      <c r="R105" s="2"/>
+      <c r="S105" s="2"/>
+      <c r="T105" s="2"/>
+      <c r="U105" s="2"/>
+      <c r="V105" s="2"/>
+      <c r="W105" s="2"/>
+      <c r="X105" s="2"/>
+      <c r="Y105" s="2"/>
     </row>
     <row r="106" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
@@ -4815,16 +4818,16 @@
         <v>105</v>
       </c>
       <c r="C106" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G106" s="2"/>
       <c r="H106" s="2"/>
@@ -4846,44 +4849,44 @@
       <c r="X106" s="2"/>
       <c r="Y106" s="2"/>
     </row>
-    <row r="107" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A107" s="2" t="s">
+    <row r="107" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="13" t="s">
         <v>49</v>
       </c>
       <c r="B107" s="2">
         <v>106</v>
       </c>
-      <c r="C107" s="5" t="s">
+      <c r="C107" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D107" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E107" s="2" t="s">
+      <c r="D107" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E107" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F107" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G107" s="2"/>
-      <c r="H107" s="2"/>
-      <c r="I107" s="2"/>
-      <c r="J107" s="2"/>
-      <c r="K107" s="2"/>
-      <c r="L107" s="2"/>
-      <c r="M107" s="2"/>
-      <c r="N107" s="2"/>
-      <c r="O107" s="2"/>
-      <c r="P107" s="2"/>
-      <c r="Q107" s="2"/>
-      <c r="R107" s="2"/>
-      <c r="S107" s="2"/>
-      <c r="T107" s="2"/>
-      <c r="U107" s="2"/>
-      <c r="V107" s="2"/>
-      <c r="W107" s="2"/>
-      <c r="X107" s="2"/>
-      <c r="Y107" s="2"/>
+      <c r="F107" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G107" s="13"/>
+      <c r="H107" s="13"/>
+      <c r="I107" s="13"/>
+      <c r="J107" s="13"/>
+      <c r="K107" s="13"/>
+      <c r="L107" s="13"/>
+      <c r="M107" s="13"/>
+      <c r="N107" s="13"/>
+      <c r="O107" s="13"/>
+      <c r="P107" s="13"/>
+      <c r="Q107" s="13"/>
+      <c r="R107" s="13"/>
+      <c r="S107" s="13"/>
+      <c r="T107" s="13"/>
+      <c r="U107" s="13"/>
+      <c r="V107" s="13"/>
+      <c r="W107" s="13"/>
+      <c r="X107" s="13"/>
+      <c r="Y107" s="13"/>
     </row>
     <row r="108" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
@@ -4896,7 +4899,7 @@
         <v>7</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>9</v>
@@ -4935,7 +4938,7 @@
         <v>7</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>9</v>
@@ -4974,7 +4977,7 @@
         <v>7</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>9</v>
@@ -5003,101 +5006,101 @@
       <c r="Y110" s="2"/>
     </row>
     <row r="111" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A111" s="3" t="s">
+      <c r="A111" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B111" s="2">
         <v>110</v>
       </c>
-      <c r="C111" s="3" t="s">
+      <c r="C111" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D111" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="E111" s="3" t="s">
+      <c r="D111" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E111" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F111" s="6" t="s">
+      <c r="F111" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G111" s="3"/>
-      <c r="H111" s="3"/>
-      <c r="I111" s="3"/>
-      <c r="J111" s="3"/>
-      <c r="K111" s="3"/>
-      <c r="L111" s="3"/>
-      <c r="M111" s="3"/>
-      <c r="N111" s="3"/>
-      <c r="O111" s="3"/>
-      <c r="P111" s="3"/>
-      <c r="Q111" s="3"/>
-      <c r="R111" s="3"/>
-      <c r="S111" s="3"/>
-      <c r="T111" s="3"/>
-      <c r="U111" s="3"/>
-      <c r="V111" s="3"/>
-      <c r="W111" s="3"/>
-      <c r="X111" s="3"/>
-      <c r="Y111" s="3"/>
+      <c r="G111" s="2"/>
+      <c r="H111" s="2"/>
+      <c r="I111" s="2"/>
+      <c r="J111" s="2"/>
+      <c r="K111" s="2"/>
+      <c r="L111" s="2"/>
+      <c r="M111" s="2"/>
+      <c r="N111" s="2"/>
+      <c r="O111" s="2"/>
+      <c r="P111" s="2"/>
+      <c r="Q111" s="2"/>
+      <c r="R111" s="2"/>
+      <c r="S111" s="2"/>
+      <c r="T111" s="2"/>
+      <c r="U111" s="2"/>
+      <c r="V111" s="2"/>
+      <c r="W111" s="2"/>
+      <c r="X111" s="2"/>
+      <c r="Y111" s="2"/>
     </row>
     <row r="112" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A112" s="3" t="s">
+      <c r="A112" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B112" s="2">
         <v>111</v>
       </c>
-      <c r="C112" s="3" t="s">
+      <c r="C112" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D112" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E112" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F112" s="6" t="s">
+      <c r="D112" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F112" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G112" s="3"/>
-      <c r="H112" s="3"/>
-      <c r="I112" s="3"/>
-      <c r="J112" s="3"/>
-      <c r="K112" s="3"/>
-      <c r="L112" s="3"/>
-      <c r="M112" s="3"/>
-      <c r="N112" s="3"/>
-      <c r="O112" s="3"/>
-      <c r="P112" s="3"/>
-      <c r="Q112" s="3"/>
-      <c r="R112" s="3"/>
-      <c r="S112" s="3"/>
-      <c r="T112" s="3"/>
-      <c r="U112" s="3"/>
-      <c r="V112" s="3"/>
-      <c r="W112" s="3"/>
-      <c r="X112" s="3"/>
-      <c r="Y112" s="3"/>
+      <c r="G112" s="2"/>
+      <c r="H112" s="2"/>
+      <c r="I112" s="2"/>
+      <c r="J112" s="2"/>
+      <c r="K112" s="2"/>
+      <c r="L112" s="2"/>
+      <c r="M112" s="2"/>
+      <c r="N112" s="2"/>
+      <c r="O112" s="2"/>
+      <c r="P112" s="2"/>
+      <c r="Q112" s="2"/>
+      <c r="R112" s="2"/>
+      <c r="S112" s="2"/>
+      <c r="T112" s="2"/>
+      <c r="U112" s="2"/>
+      <c r="V112" s="2"/>
+      <c r="W112" s="2"/>
+      <c r="X112" s="2"/>
+      <c r="Y112" s="2"/>
     </row>
     <row r="113" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A113" s="2" t="s">
-        <v>70</v>
+      <c r="A113" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="B113" s="2">
         <v>112</v>
       </c>
-      <c r="C113" s="2" t="s">
+      <c r="C113" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D113" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E113" s="2" t="s">
+      <c r="D113" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E113" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F113" s="2" t="s">
-        <v>10</v>
+      <c r="F113" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="G113" s="3"/>
       <c r="H113" s="3"/>
@@ -5120,22 +5123,22 @@
       <c r="Y113" s="3"/>
     </row>
     <row r="114" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A114" s="2" t="s">
-        <v>70</v>
+      <c r="A114" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="B114" s="2">
         <v>113</v>
       </c>
-      <c r="C114" s="2" t="s">
+      <c r="C114" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D114" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E114" s="2" t="s">
+      <c r="D114" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="E114" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F114" s="2" t="s">
+      <c r="F114" s="6" t="s">
         <v>19</v>
       </c>
       <c r="G114" s="3"/>
@@ -5159,22 +5162,22 @@
       <c r="Y114" s="3"/>
     </row>
     <row r="115" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A115" s="2" t="s">
-        <v>70</v>
+      <c r="A115" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="B115" s="2">
         <v>114</v>
       </c>
-      <c r="C115" s="2" t="s">
+      <c r="C115" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D115" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E115" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F115" s="2" t="s">
+      <c r="D115" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E115" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="F115" s="6" t="s">
         <v>19</v>
       </c>
       <c r="G115" s="3"/>
@@ -5205,16 +5208,16 @@
         <v>115</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D116" s="10" t="s">
-        <v>88</v>
+        <v>7</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G116" s="3"/>
       <c r="H116" s="3"/>
@@ -5244,13 +5247,13 @@
         <v>116</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F117" s="2" t="s">
         <v>19</v>
@@ -5286,7 +5289,7 @@
         <v>11</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>17</v>
@@ -5324,8 +5327,8 @@
       <c r="C119" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D119" s="3" t="s">
-        <v>22</v>
+      <c r="D119" s="10" t="s">
+        <v>88</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>17</v>
@@ -5364,7 +5367,7 @@
         <v>11</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>17</v>
@@ -5403,7 +5406,7 @@
         <v>11</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E121" s="2" t="s">
         <v>17</v>
@@ -5439,13 +5442,13 @@
         <v>121</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="E122" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F122" s="2" t="s">
         <v>19</v>
@@ -5481,10 +5484,10 @@
         <v>11</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="E123" s="2" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="F123" s="2" t="s">
         <v>19</v>
@@ -5520,10 +5523,10 @@
         <v>11</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="F124" s="2" t="s">
         <v>19</v>
@@ -5556,13 +5559,13 @@
         <v>124</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="F125" s="2" t="s">
         <v>19</v>
@@ -5594,11 +5597,11 @@
       <c r="B126" s="2">
         <v>125</v>
       </c>
-      <c r="C126" s="5" t="s">
+      <c r="C126" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>51</v>
@@ -5633,11 +5636,11 @@
       <c r="B127" s="2">
         <v>126</v>
       </c>
-      <c r="C127" s="5" t="s">
+      <c r="C127" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E127" s="2" t="s">
         <v>51</v>
@@ -5673,16 +5676,16 @@
         <v>127</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="E128" s="2" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G128" s="3"/>
       <c r="H128" s="3"/>
@@ -5711,17 +5714,17 @@
       <c r="B129" s="2">
         <v>128</v>
       </c>
-      <c r="C129" s="2" t="s">
-        <v>7</v>
+      <c r="C129" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="E129" s="2" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="F129" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G129" s="3"/>
       <c r="H129" s="3"/>
@@ -5754,10 +5757,10 @@
         <v>11</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="E130" s="2" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="F130" s="2" t="s">
         <v>19</v>
@@ -5789,17 +5792,17 @@
       <c r="B131" s="2">
         <v>130</v>
       </c>
-      <c r="C131" s="5" t="s">
-        <v>11</v>
+      <c r="C131" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E131" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="F131" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G131" s="3"/>
       <c r="H131" s="3"/>
@@ -5828,17 +5831,17 @@
       <c r="B132" s="2">
         <v>131</v>
       </c>
-      <c r="C132" s="5" t="s">
-        <v>11</v>
+      <c r="C132" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G132" s="3"/>
       <c r="H132" s="3"/>
@@ -5868,16 +5871,16 @@
         <v>132</v>
       </c>
       <c r="C133" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="E133" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F133" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G133" s="3"/>
       <c r="H133" s="3"/>
@@ -5910,13 +5913,13 @@
         <v>11</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G134" s="3"/>
       <c r="H134" s="3"/>
@@ -5949,13 +5952,13 @@
         <v>11</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="E135" s="2" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="F135" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G135" s="3"/>
       <c r="H135" s="3"/>
@@ -5985,16 +5988,16 @@
         <v>135</v>
       </c>
       <c r="C136" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E136" s="2" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="F136" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G136" s="3"/>
       <c r="H136" s="3"/>
@@ -6027,33 +6030,33 @@
         <v>11</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E137" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F137" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G137" s="2"/>
-      <c r="H137" s="2"/>
-      <c r="I137" s="2"/>
-      <c r="J137" s="2"/>
-      <c r="K137" s="2"/>
-      <c r="L137" s="2"/>
-      <c r="M137" s="2"/>
-      <c r="N137" s="2"/>
-      <c r="O137" s="2"/>
-      <c r="P137" s="2"/>
-      <c r="Q137" s="2"/>
-      <c r="R137" s="2"/>
-      <c r="S137" s="2"/>
-      <c r="T137" s="2"/>
-      <c r="U137" s="2"/>
-      <c r="V137" s="2"/>
-      <c r="W137" s="2"/>
-      <c r="X137" s="2"/>
-      <c r="Y137" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="G137" s="3"/>
+      <c r="H137" s="3"/>
+      <c r="I137" s="3"/>
+      <c r="J137" s="3"/>
+      <c r="K137" s="3"/>
+      <c r="L137" s="3"/>
+      <c r="M137" s="3"/>
+      <c r="N137" s="3"/>
+      <c r="O137" s="3"/>
+      <c r="P137" s="3"/>
+      <c r="Q137" s="3"/>
+      <c r="R137" s="3"/>
+      <c r="S137" s="3"/>
+      <c r="T137" s="3"/>
+      <c r="U137" s="3"/>
+      <c r="V137" s="3"/>
+      <c r="W137" s="3"/>
+      <c r="X137" s="3"/>
+      <c r="Y137" s="3"/>
     </row>
     <row r="138" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
@@ -6066,7 +6069,7 @@
         <v>11</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E138" s="2" t="s">
         <v>57</v>
@@ -6074,25 +6077,25 @@
       <c r="F138" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G138" s="2"/>
-      <c r="H138" s="2"/>
-      <c r="I138" s="2"/>
-      <c r="J138" s="2"/>
-      <c r="K138" s="2"/>
-      <c r="L138" s="2"/>
-      <c r="M138" s="2"/>
-      <c r="N138" s="2"/>
-      <c r="O138" s="2"/>
-      <c r="P138" s="2"/>
-      <c r="Q138" s="2"/>
-      <c r="R138" s="2"/>
-      <c r="S138" s="2"/>
-      <c r="T138" s="2"/>
-      <c r="U138" s="2"/>
-      <c r="V138" s="2"/>
-      <c r="W138" s="2"/>
-      <c r="X138" s="2"/>
-      <c r="Y138" s="2"/>
+      <c r="G138" s="3"/>
+      <c r="H138" s="3"/>
+      <c r="I138" s="3"/>
+      <c r="J138" s="3"/>
+      <c r="K138" s="3"/>
+      <c r="L138" s="3"/>
+      <c r="M138" s="3"/>
+      <c r="N138" s="3"/>
+      <c r="O138" s="3"/>
+      <c r="P138" s="3"/>
+      <c r="Q138" s="3"/>
+      <c r="R138" s="3"/>
+      <c r="S138" s="3"/>
+      <c r="T138" s="3"/>
+      <c r="U138" s="3"/>
+      <c r="V138" s="3"/>
+      <c r="W138" s="3"/>
+      <c r="X138" s="3"/>
+      <c r="Y138" s="3"/>
     </row>
     <row r="139" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
@@ -6105,7 +6108,7 @@
         <v>11</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E139" s="2" t="s">
         <v>57</v>
@@ -6113,25 +6116,25 @@
       <c r="F139" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G139" s="2"/>
-      <c r="H139" s="2"/>
-      <c r="I139" s="2"/>
-      <c r="J139" s="2"/>
-      <c r="K139" s="2"/>
-      <c r="L139" s="2"/>
-      <c r="M139" s="2"/>
-      <c r="N139" s="2"/>
-      <c r="O139" s="2"/>
-      <c r="P139" s="2"/>
-      <c r="Q139" s="2"/>
-      <c r="R139" s="2"/>
-      <c r="S139" s="2"/>
-      <c r="T139" s="2"/>
-      <c r="U139" s="2"/>
-      <c r="V139" s="2"/>
-      <c r="W139" s="2"/>
-      <c r="X139" s="2"/>
-      <c r="Y139" s="2"/>
+      <c r="G139" s="3"/>
+      <c r="H139" s="3"/>
+      <c r="I139" s="3"/>
+      <c r="J139" s="3"/>
+      <c r="K139" s="3"/>
+      <c r="L139" s="3"/>
+      <c r="M139" s="3"/>
+      <c r="N139" s="3"/>
+      <c r="O139" s="3"/>
+      <c r="P139" s="3"/>
+      <c r="Q139" s="3"/>
+      <c r="R139" s="3"/>
+      <c r="S139" s="3"/>
+      <c r="T139" s="3"/>
+      <c r="U139" s="3"/>
+      <c r="V139" s="3"/>
+      <c r="W139" s="3"/>
+      <c r="X139" s="3"/>
+      <c r="Y139" s="3"/>
     </row>
     <row r="140" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
@@ -6144,7 +6147,7 @@
         <v>11</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E140" s="2" t="s">
         <v>57</v>
@@ -6183,7 +6186,7 @@
         <v>11</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="E141" s="2" t="s">
         <v>57</v>
@@ -6222,13 +6225,13 @@
         <v>11</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E142" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F142" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G142" s="2"/>
       <c r="H142" s="2"/>
@@ -6257,17 +6260,17 @@
       <c r="B143" s="2">
         <v>142</v>
       </c>
-      <c r="C143" s="2" t="s">
-        <v>7</v>
+      <c r="C143" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E143" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F143" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G143" s="2"/>
       <c r="H143" s="2"/>
@@ -6297,16 +6300,16 @@
         <v>143</v>
       </c>
       <c r="C144" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D144" s="10" t="s">
-        <v>89</v>
+        <v>11</v>
+      </c>
+      <c r="D144" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="E144" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F144" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G144" s="2"/>
       <c r="H144" s="2"/>
@@ -6336,16 +6339,16 @@
         <v>144</v>
       </c>
       <c r="C145" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E145" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F145" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G145" s="2"/>
       <c r="H145" s="2"/>
@@ -6377,14 +6380,14 @@
       <c r="C146" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D146" s="10" t="s">
-        <v>67</v>
+      <c r="D146" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="E146" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F146" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G146" s="2"/>
       <c r="H146" s="2"/>
@@ -6416,8 +6419,8 @@
       <c r="C147" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D147" s="3" t="s">
-        <v>68</v>
+      <c r="D147" s="10" t="s">
+        <v>89</v>
       </c>
       <c r="E147" s="2" t="s">
         <v>9</v>
@@ -6456,7 +6459,7 @@
         <v>7</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E148" s="2" t="s">
         <v>9</v>
@@ -6491,17 +6494,17 @@
       <c r="B149" s="2">
         <v>148</v>
       </c>
-      <c r="C149" s="5" t="s">
-        <v>11</v>
+      <c r="C149" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D149" s="10" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="E149" s="2" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="F149" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G149" s="2"/>
       <c r="H149" s="2"/>
@@ -6524,12 +6527,24 @@
       <c r="Y149" s="2"/>
     </row>
     <row r="150" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A150" s="2"/>
-      <c r="B150" s="2"/>
-      <c r="C150" s="5"/>
-      <c r="D150" s="3"/>
-      <c r="E150" s="2"/>
-      <c r="F150" s="2"/>
+      <c r="A150" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B150" s="2">
+        <v>149</v>
+      </c>
+      <c r="C150" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D150" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E150" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F150" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="G150" s="2"/>
       <c r="H150" s="2"/>
       <c r="I150" s="2"/>
@@ -6551,12 +6566,24 @@
       <c r="Y150" s="2"/>
     </row>
     <row r="151" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A151" s="2"/>
-      <c r="B151" s="2"/>
-      <c r="C151" s="5"/>
-      <c r="D151" s="3"/>
-      <c r="E151" s="2"/>
-      <c r="F151" s="2"/>
+      <c r="A151" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B151" s="2">
+        <v>150</v>
+      </c>
+      <c r="C151" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D151" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E151" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F151" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="G151" s="2"/>
       <c r="H151" s="2"/>
       <c r="I151" s="2"/>
@@ -6578,12 +6605,24 @@
       <c r="Y151" s="2"/>
     </row>
     <row r="152" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A152" s="2"/>
-      <c r="B152" s="2"/>
-      <c r="C152" s="5"/>
-      <c r="D152" s="3"/>
-      <c r="E152" s="2"/>
-      <c r="F152" s="2"/>
+      <c r="A152" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B152" s="2">
+        <v>151</v>
+      </c>
+      <c r="C152" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D152" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E152" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F152" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="G152" s="2"/>
       <c r="H152" s="2"/>
       <c r="I152" s="2"/>
@@ -6661,7 +6700,7 @@
     <row r="155" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A155" s="2"/>
       <c r="B155" s="2"/>
-      <c r="C155" s="2"/>
+      <c r="C155" s="5"/>
       <c r="D155" s="3"/>
       <c r="E155" s="2"/>
       <c r="F155" s="2"/>
@@ -6742,7 +6781,7 @@
     <row r="158" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A158" s="2"/>
       <c r="B158" s="2"/>
-      <c r="C158" s="5"/>
+      <c r="C158" s="2"/>
       <c r="D158" s="3"/>
       <c r="E158" s="2"/>
       <c r="F158" s="2"/>
@@ -6796,8 +6835,8 @@
     <row r="160" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A160" s="2"/>
       <c r="B160" s="2"/>
-      <c r="C160" s="2"/>
-      <c r="D160" s="2"/>
+      <c r="C160" s="5"/>
+      <c r="D160" s="3"/>
       <c r="E160" s="2"/>
       <c r="F160" s="2"/>
       <c r="G160" s="2"/>
@@ -6823,8 +6862,8 @@
     <row r="161" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A161" s="2"/>
       <c r="B161" s="2"/>
-      <c r="C161" s="2"/>
-      <c r="D161" s="2"/>
+      <c r="C161" s="5"/>
+      <c r="D161" s="3"/>
       <c r="E161" s="2"/>
       <c r="F161" s="2"/>
       <c r="G161" s="2"/>
@@ -6850,8 +6889,8 @@
     <row r="162" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A162" s="2"/>
       <c r="B162" s="2"/>
-      <c r="C162" s="2"/>
-      <c r="D162" s="2"/>
+      <c r="C162" s="5"/>
+      <c r="D162" s="3"/>
       <c r="E162" s="2"/>
       <c r="F162" s="2"/>
       <c r="G162" s="2"/>
@@ -28285,6 +28324,87 @@
       <c r="X955" s="2"/>
       <c r="Y955" s="2"/>
     </row>
+    <row r="956" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A956" s="2"/>
+      <c r="B956" s="2"/>
+      <c r="C956" s="2"/>
+      <c r="D956" s="2"/>
+      <c r="E956" s="2"/>
+      <c r="F956" s="2"/>
+      <c r="G956" s="2"/>
+      <c r="H956" s="2"/>
+      <c r="I956" s="2"/>
+      <c r="J956" s="2"/>
+      <c r="K956" s="2"/>
+      <c r="L956" s="2"/>
+      <c r="M956" s="2"/>
+      <c r="N956" s="2"/>
+      <c r="O956" s="2"/>
+      <c r="P956" s="2"/>
+      <c r="Q956" s="2"/>
+      <c r="R956" s="2"/>
+      <c r="S956" s="2"/>
+      <c r="T956" s="2"/>
+      <c r="U956" s="2"/>
+      <c r="V956" s="2"/>
+      <c r="W956" s="2"/>
+      <c r="X956" s="2"/>
+      <c r="Y956" s="2"/>
+    </row>
+    <row r="957" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A957" s="2"/>
+      <c r="B957" s="2"/>
+      <c r="C957" s="2"/>
+      <c r="D957" s="2"/>
+      <c r="E957" s="2"/>
+      <c r="F957" s="2"/>
+      <c r="G957" s="2"/>
+      <c r="H957" s="2"/>
+      <c r="I957" s="2"/>
+      <c r="J957" s="2"/>
+      <c r="K957" s="2"/>
+      <c r="L957" s="2"/>
+      <c r="M957" s="2"/>
+      <c r="N957" s="2"/>
+      <c r="O957" s="2"/>
+      <c r="P957" s="2"/>
+      <c r="Q957" s="2"/>
+      <c r="R957" s="2"/>
+      <c r="S957" s="2"/>
+      <c r="T957" s="2"/>
+      <c r="U957" s="2"/>
+      <c r="V957" s="2"/>
+      <c r="W957" s="2"/>
+      <c r="X957" s="2"/>
+      <c r="Y957" s="2"/>
+    </row>
+    <row r="958" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A958" s="2"/>
+      <c r="B958" s="2"/>
+      <c r="C958" s="2"/>
+      <c r="D958" s="2"/>
+      <c r="E958" s="2"/>
+      <c r="F958" s="2"/>
+      <c r="G958" s="2"/>
+      <c r="H958" s="2"/>
+      <c r="I958" s="2"/>
+      <c r="J958" s="2"/>
+      <c r="K958" s="2"/>
+      <c r="L958" s="2"/>
+      <c r="M958" s="2"/>
+      <c r="N958" s="2"/>
+      <c r="O958" s="2"/>
+      <c r="P958" s="2"/>
+      <c r="Q958" s="2"/>
+      <c r="R958" s="2"/>
+      <c r="S958" s="2"/>
+      <c r="T958" s="2"/>
+      <c r="U958" s="2"/>
+      <c r="V958" s="2"/>
+      <c r="W958" s="2"/>
+      <c r="X958" s="2"/>
+      <c r="Y958" s="2"/>
+    </row>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{49968090-594F-4035-ABCC-088176AC5527}" filter="1" showAutoFilter="1">
@@ -28292,7 +28412,7 @@
       <autoFilter ref="A1:A950"/>
     </customSheetView>
   </customSheetViews>
-  <conditionalFormatting sqref="G1 F1:F955">
+  <conditionalFormatting sqref="G1 F1:F958">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Read">
       <formula>NOT(ISERROR(SEARCH(("Read"),(F1))))</formula>
     </cfRule>
@@ -28304,6 +28424,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
@@ -28315,13 +28436,13 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>ScreenIds!$B$2:$B$72</xm:f>
+            <xm:f>ScreenIds!$B$2:$B$73</xm:f>
           </x14:formula1>
           <xm:sqref>E1:E1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>ScreenIds!$B$3:$B$72</xm:f>
+            <xm:f>ScreenIds!$B$3:$B$73</xm:f>
           </x14:formula1>
           <xm:sqref>D1:D1048576</xm:sqref>
         </x14:dataValidation>
@@ -28350,8 +28471,8 @@
   </sheetPr>
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -28940,7 +29061,9 @@
       </c>
     </row>
     <row r="73" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="8"/>
+      <c r="B73" s="8" t="s">
+        <v>90</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated permissions for Customer Admin Service Plus Software Layer.
</commit_message>
<xml_diff>
--- a/Roles and Permissions.xlsx
+++ b/Roles and Permissions.xlsx
@@ -16,7 +16,7 @@
     <sheet name="ScreenIds" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Z_49968090_594F_4035_ABCC_088176AC5527_.wvu.FilterData" localSheetId="0" hidden="1">'Roles and Permissions'!$A$1:$A$958</definedName>
+    <definedName name="Z_49968090_594F_4035_ABCC_088176AC5527_.wvu.FilterData" localSheetId="0" hidden="1">'Roles and Permissions'!$A$1:$A$961</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <customWorkbookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="91">
   <si>
     <t>User</t>
   </si>
@@ -700,17 +700,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Y958"/>
+  <dimension ref="A1:Y961"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C156" sqref="C156"/>
+    <sheetView tabSelected="1" topLeftCell="A149" workbookViewId="0">
+      <selection activeCell="E163" sqref="E163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.6640625" customWidth="1"/>
     <col min="2" max="2" width="17.44140625" customWidth="1"/>
-    <col min="4" max="4" width="34" customWidth="1"/>
+    <col min="4" max="4" width="37.77734375" customWidth="1"/>
     <col min="5" max="5" width="30.21875" customWidth="1"/>
     <col min="6" max="6" width="12.44140625" customWidth="1"/>
   </cols>
@@ -3601,7 +3601,7 @@
       <c r="X74" s="2"/>
       <c r="Y74" s="2"/>
     </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>44</v>
       </c>
@@ -3615,7 +3615,7 @@
         <v>35</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="F75" s="2" t="s">
         <v>19</v>
@@ -3640,7 +3640,7 @@
       <c r="X75" s="2"/>
       <c r="Y75" s="2"/>
     </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>44</v>
       </c>
@@ -3679,21 +3679,21 @@
       <c r="X76" s="2"/>
       <c r="Y76" s="2"/>
     </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B77" s="2">
         <v>76</v>
       </c>
-      <c r="C77" s="2" t="s">
-        <v>7</v>
+      <c r="C77" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>10</v>
@@ -3720,19 +3720,19 @@
     </row>
     <row r="78" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B78" s="2">
         <v>77</v>
       </c>
-      <c r="C78" s="2" t="s">
-        <v>7</v>
+      <c r="C78" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="F78" s="2" t="s">
         <v>19</v>
@@ -3759,22 +3759,22 @@
     </row>
     <row r="79" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B79" s="2">
         <v>78</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="C79" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
@@ -3804,16 +3804,16 @@
         <v>79</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
@@ -3843,13 +3843,13 @@
         <v>80</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F81" s="2" t="s">
         <v>19</v>
@@ -3885,7 +3885,7 @@
         <v>11</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>17</v>
@@ -3924,7 +3924,7 @@
         <v>11</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>22</v>
+        <v>88</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>17</v>
@@ -3963,7 +3963,7 @@
         <v>11</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>17</v>
@@ -4002,7 +4002,7 @@
         <v>11</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>17</v>
@@ -4038,13 +4038,13 @@
         <v>85</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F86" s="2" t="s">
         <v>19</v>
@@ -4080,10 +4080,10 @@
         <v>11</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="F87" s="2" t="s">
         <v>19</v>
@@ -4119,10 +4119,10 @@
         <v>11</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="F88" s="2" t="s">
         <v>19</v>
@@ -4155,13 +4155,13 @@
         <v>88</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="F89" s="2" t="s">
         <v>19</v>
@@ -4193,11 +4193,11 @@
       <c r="B90" s="2">
         <v>89</v>
       </c>
-      <c r="C90" s="5" t="s">
+      <c r="C90" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>51</v>
@@ -4232,11 +4232,11 @@
       <c r="B91" s="2">
         <v>90</v>
       </c>
-      <c r="C91" s="5" t="s">
+      <c r="C91" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>51</v>
@@ -4272,16 +4272,16 @@
         <v>91</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
@@ -4310,17 +4310,17 @@
       <c r="B93" s="2">
         <v>92</v>
       </c>
-      <c r="C93" s="2" t="s">
-        <v>7</v>
+      <c r="C93" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
@@ -4353,10 +4353,10 @@
         <v>11</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="F94" s="2" t="s">
         <v>19</v>
@@ -4388,17 +4388,17 @@
       <c r="B95" s="2">
         <v>94</v>
       </c>
-      <c r="C95" s="5" t="s">
-        <v>11</v>
+      <c r="C95" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
@@ -4427,17 +4427,17 @@
       <c r="B96" s="2">
         <v>95</v>
       </c>
-      <c r="C96" s="5" t="s">
-        <v>11</v>
+      <c r="C96" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
@@ -4467,16 +4467,16 @@
         <v>96</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
@@ -4509,13 +4509,13 @@
         <v>11</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
@@ -4548,13 +4548,13 @@
         <v>11</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
@@ -4584,16 +4584,16 @@
         <v>99</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G100" s="2"/>
       <c r="H100" s="2"/>
@@ -4626,13 +4626,13 @@
         <v>11</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G101" s="2"/>
       <c r="H101" s="2"/>
@@ -4665,7 +4665,7 @@
         <v>11</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>57</v>
@@ -4704,7 +4704,7 @@
         <v>11</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>57</v>
@@ -4743,7 +4743,7 @@
         <v>11</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E104" s="2" t="s">
         <v>57</v>
@@ -4782,7 +4782,7 @@
         <v>11</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>57</v>
@@ -4821,13 +4821,13 @@
         <v>11</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G106" s="2"/>
       <c r="H106" s="2"/>
@@ -4849,44 +4849,44 @@
       <c r="X106" s="2"/>
       <c r="Y106" s="2"/>
     </row>
-    <row r="107" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="13" t="s">
+    <row r="107" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B107" s="2">
         <v>106</v>
       </c>
-      <c r="C107" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D107" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="E107" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F107" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G107" s="13"/>
-      <c r="H107" s="13"/>
-      <c r="I107" s="13"/>
-      <c r="J107" s="13"/>
-      <c r="K107" s="13"/>
-      <c r="L107" s="13"/>
-      <c r="M107" s="13"/>
-      <c r="N107" s="13"/>
-      <c r="O107" s="13"/>
-      <c r="P107" s="13"/>
-      <c r="Q107" s="13"/>
-      <c r="R107" s="13"/>
-      <c r="S107" s="13"/>
-      <c r="T107" s="13"/>
-      <c r="U107" s="13"/>
-      <c r="V107" s="13"/>
-      <c r="W107" s="13"/>
-      <c r="X107" s="13"/>
-      <c r="Y107" s="13"/>
+      <c r="C107" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F107" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G107" s="2"/>
+      <c r="H107" s="2"/>
+      <c r="I107" s="2"/>
+      <c r="J107" s="2"/>
+      <c r="K107" s="2"/>
+      <c r="L107" s="2"/>
+      <c r="M107" s="2"/>
+      <c r="N107" s="2"/>
+      <c r="O107" s="2"/>
+      <c r="P107" s="2"/>
+      <c r="Q107" s="2"/>
+      <c r="R107" s="2"/>
+      <c r="S107" s="2"/>
+      <c r="T107" s="2"/>
+      <c r="U107" s="2"/>
+      <c r="V107" s="2"/>
+      <c r="W107" s="2"/>
+      <c r="X107" s="2"/>
+      <c r="Y107" s="2"/>
     </row>
     <row r="108" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
@@ -4896,16 +4896,16 @@
         <v>107</v>
       </c>
       <c r="C108" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>88</v>
+        <v>34</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G108" s="2"/>
       <c r="H108" s="2"/>
@@ -4935,16 +4935,16 @@
         <v>108</v>
       </c>
       <c r="C109" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G109" s="2"/>
       <c r="H109" s="2"/>
@@ -4966,44 +4966,44 @@
       <c r="X109" s="2"/>
       <c r="Y109" s="2"/>
     </row>
-    <row r="110" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A110" s="2" t="s">
+    <row r="110" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="13" t="s">
         <v>49</v>
       </c>
       <c r="B110" s="2">
         <v>109</v>
       </c>
-      <c r="C110" s="5" t="s">
+      <c r="C110" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D110" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E110" s="2" t="s">
+      <c r="D110" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E110" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F110" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G110" s="2"/>
-      <c r="H110" s="2"/>
-      <c r="I110" s="2"/>
-      <c r="J110" s="2"/>
-      <c r="K110" s="2"/>
-      <c r="L110" s="2"/>
-      <c r="M110" s="2"/>
-      <c r="N110" s="2"/>
-      <c r="O110" s="2"/>
-      <c r="P110" s="2"/>
-      <c r="Q110" s="2"/>
-      <c r="R110" s="2"/>
-      <c r="S110" s="2"/>
-      <c r="T110" s="2"/>
-      <c r="U110" s="2"/>
-      <c r="V110" s="2"/>
-      <c r="W110" s="2"/>
-      <c r="X110" s="2"/>
-      <c r="Y110" s="2"/>
+      <c r="F110" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G110" s="13"/>
+      <c r="H110" s="13"/>
+      <c r="I110" s="13"/>
+      <c r="J110" s="13"/>
+      <c r="K110" s="13"/>
+      <c r="L110" s="13"/>
+      <c r="M110" s="13"/>
+      <c r="N110" s="13"/>
+      <c r="O110" s="13"/>
+      <c r="P110" s="13"/>
+      <c r="Q110" s="13"/>
+      <c r="R110" s="13"/>
+      <c r="S110" s="13"/>
+      <c r="T110" s="13"/>
+      <c r="U110" s="13"/>
+      <c r="V110" s="13"/>
+      <c r="W110" s="13"/>
+      <c r="X110" s="13"/>
+      <c r="Y110" s="13"/>
     </row>
     <row r="111" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
@@ -5016,7 +5016,7 @@
         <v>7</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>9</v>
@@ -5055,7 +5055,7 @@
         <v>7</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>9</v>
@@ -5084,140 +5084,140 @@
       <c r="Y112" s="2"/>
     </row>
     <row r="113" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A113" s="3" t="s">
+      <c r="A113" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B113" s="2">
         <v>112</v>
       </c>
-      <c r="C113" s="3" t="s">
+      <c r="C113" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D113" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="E113" s="3" t="s">
+      <c r="D113" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E113" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F113" s="6" t="s">
+      <c r="F113" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G113" s="3"/>
-      <c r="H113" s="3"/>
-      <c r="I113" s="3"/>
-      <c r="J113" s="3"/>
-      <c r="K113" s="3"/>
-      <c r="L113" s="3"/>
-      <c r="M113" s="3"/>
-      <c r="N113" s="3"/>
-      <c r="O113" s="3"/>
-      <c r="P113" s="3"/>
-      <c r="Q113" s="3"/>
-      <c r="R113" s="3"/>
-      <c r="S113" s="3"/>
-      <c r="T113" s="3"/>
-      <c r="U113" s="3"/>
-      <c r="V113" s="3"/>
-      <c r="W113" s="3"/>
-      <c r="X113" s="3"/>
-      <c r="Y113" s="3"/>
+      <c r="G113" s="2"/>
+      <c r="H113" s="2"/>
+      <c r="I113" s="2"/>
+      <c r="J113" s="2"/>
+      <c r="K113" s="2"/>
+      <c r="L113" s="2"/>
+      <c r="M113" s="2"/>
+      <c r="N113" s="2"/>
+      <c r="O113" s="2"/>
+      <c r="P113" s="2"/>
+      <c r="Q113" s="2"/>
+      <c r="R113" s="2"/>
+      <c r="S113" s="2"/>
+      <c r="T113" s="2"/>
+      <c r="U113" s="2"/>
+      <c r="V113" s="2"/>
+      <c r="W113" s="2"/>
+      <c r="X113" s="2"/>
+      <c r="Y113" s="2"/>
     </row>
     <row r="114" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A114" s="3" t="s">
+      <c r="A114" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B114" s="2">
         <v>113</v>
       </c>
-      <c r="C114" s="3" t="s">
+      <c r="C114" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D114" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="E114" s="3" t="s">
+      <c r="D114" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E114" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F114" s="6" t="s">
+      <c r="F114" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G114" s="3"/>
-      <c r="H114" s="3"/>
-      <c r="I114" s="3"/>
-      <c r="J114" s="3"/>
-      <c r="K114" s="3"/>
-      <c r="L114" s="3"/>
-      <c r="M114" s="3"/>
-      <c r="N114" s="3"/>
-      <c r="O114" s="3"/>
-      <c r="P114" s="3"/>
-      <c r="Q114" s="3"/>
-      <c r="R114" s="3"/>
-      <c r="S114" s="3"/>
-      <c r="T114" s="3"/>
-      <c r="U114" s="3"/>
-      <c r="V114" s="3"/>
-      <c r="W114" s="3"/>
-      <c r="X114" s="3"/>
-      <c r="Y114" s="3"/>
+      <c r="G114" s="2"/>
+      <c r="H114" s="2"/>
+      <c r="I114" s="2"/>
+      <c r="J114" s="2"/>
+      <c r="K114" s="2"/>
+      <c r="L114" s="2"/>
+      <c r="M114" s="2"/>
+      <c r="N114" s="2"/>
+      <c r="O114" s="2"/>
+      <c r="P114" s="2"/>
+      <c r="Q114" s="2"/>
+      <c r="R114" s="2"/>
+      <c r="S114" s="2"/>
+      <c r="T114" s="2"/>
+      <c r="U114" s="2"/>
+      <c r="V114" s="2"/>
+      <c r="W114" s="2"/>
+      <c r="X114" s="2"/>
+      <c r="Y114" s="2"/>
     </row>
     <row r="115" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A115" s="3" t="s">
+      <c r="A115" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B115" s="2">
         <v>114</v>
       </c>
-      <c r="C115" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D115" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E115" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="F115" s="6" t="s">
+      <c r="C115" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F115" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G115" s="3"/>
-      <c r="H115" s="3"/>
-      <c r="I115" s="3"/>
-      <c r="J115" s="3"/>
-      <c r="K115" s="3"/>
-      <c r="L115" s="3"/>
-      <c r="M115" s="3"/>
-      <c r="N115" s="3"/>
-      <c r="O115" s="3"/>
-      <c r="P115" s="3"/>
-      <c r="Q115" s="3"/>
-      <c r="R115" s="3"/>
-      <c r="S115" s="3"/>
-      <c r="T115" s="3"/>
-      <c r="U115" s="3"/>
-      <c r="V115" s="3"/>
-      <c r="W115" s="3"/>
-      <c r="X115" s="3"/>
-      <c r="Y115" s="3"/>
+      <c r="G115" s="2"/>
+      <c r="H115" s="2"/>
+      <c r="I115" s="2"/>
+      <c r="J115" s="2"/>
+      <c r="K115" s="2"/>
+      <c r="L115" s="2"/>
+      <c r="M115" s="2"/>
+      <c r="N115" s="2"/>
+      <c r="O115" s="2"/>
+      <c r="P115" s="2"/>
+      <c r="Q115" s="2"/>
+      <c r="R115" s="2"/>
+      <c r="S115" s="2"/>
+      <c r="T115" s="2"/>
+      <c r="U115" s="2"/>
+      <c r="V115" s="2"/>
+      <c r="W115" s="2"/>
+      <c r="X115" s="2"/>
+      <c r="Y115" s="2"/>
     </row>
     <row r="116" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A116" s="2" t="s">
-        <v>70</v>
+      <c r="A116" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="B116" s="2">
         <v>115</v>
       </c>
-      <c r="C116" s="2" t="s">
+      <c r="C116" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D116" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E116" s="2" t="s">
+      <c r="D116" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E116" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F116" s="2" t="s">
-        <v>10</v>
+      <c r="F116" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="G116" s="3"/>
       <c r="H116" s="3"/>
@@ -5240,22 +5240,22 @@
       <c r="Y116" s="3"/>
     </row>
     <row r="117" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A117" s="2" t="s">
-        <v>70</v>
+      <c r="A117" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="B117" s="2">
         <v>116</v>
       </c>
-      <c r="C117" s="2" t="s">
+      <c r="C117" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D117" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E117" s="2" t="s">
+      <c r="D117" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="E117" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F117" s="2" t="s">
+      <c r="F117" s="6" t="s">
         <v>19</v>
       </c>
       <c r="G117" s="3"/>
@@ -5279,22 +5279,22 @@
       <c r="Y117" s="3"/>
     </row>
     <row r="118" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A118" s="2" t="s">
-        <v>70</v>
+      <c r="A118" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="B118" s="2">
         <v>117</v>
       </c>
-      <c r="C118" s="2" t="s">
+      <c r="C118" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D118" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E118" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F118" s="2" t="s">
+      <c r="D118" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E118" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="F118" s="6" t="s">
         <v>19</v>
       </c>
       <c r="G118" s="3"/>
@@ -5325,16 +5325,16 @@
         <v>118</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D119" s="10" t="s">
-        <v>88</v>
+        <v>7</v>
+      </c>
+      <c r="D119" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G119" s="3"/>
       <c r="H119" s="3"/>
@@ -5364,13 +5364,13 @@
         <v>119</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F120" s="2" t="s">
         <v>19</v>
@@ -5406,7 +5406,7 @@
         <v>11</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E121" s="2" t="s">
         <v>17</v>
@@ -5444,8 +5444,8 @@
       <c r="C122" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D122" s="3" t="s">
-        <v>22</v>
+      <c r="D122" s="10" t="s">
+        <v>88</v>
       </c>
       <c r="E122" s="2" t="s">
         <v>17</v>
@@ -5484,7 +5484,7 @@
         <v>11</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E123" s="2" t="s">
         <v>17</v>
@@ -5523,7 +5523,7 @@
         <v>11</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E124" s="2" t="s">
         <v>17</v>
@@ -5559,13 +5559,13 @@
         <v>124</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F125" s="2" t="s">
         <v>19</v>
@@ -5601,10 +5601,10 @@
         <v>11</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="E126" s="2" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="F126" s="2" t="s">
         <v>19</v>
@@ -5640,10 +5640,10 @@
         <v>11</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="E127" s="2" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="F127" s="2" t="s">
         <v>19</v>
@@ -5676,13 +5676,13 @@
         <v>127</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E128" s="2" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="F128" s="2" t="s">
         <v>19</v>
@@ -5714,11 +5714,11 @@
       <c r="B129" s="2">
         <v>128</v>
       </c>
-      <c r="C129" s="5" t="s">
+      <c r="C129" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E129" s="2" t="s">
         <v>51</v>
@@ -5753,11 +5753,11 @@
       <c r="B130" s="2">
         <v>129</v>
       </c>
-      <c r="C130" s="5" t="s">
+      <c r="C130" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E130" s="2" t="s">
         <v>51</v>
@@ -5793,16 +5793,16 @@
         <v>130</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="E131" s="2" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="F131" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G131" s="3"/>
       <c r="H131" s="3"/>
@@ -5831,17 +5831,17 @@
       <c r="B132" s="2">
         <v>131</v>
       </c>
-      <c r="C132" s="2" t="s">
-        <v>7</v>
+      <c r="C132" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G132" s="3"/>
       <c r="H132" s="3"/>
@@ -5874,10 +5874,10 @@
         <v>11</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="E133" s="2" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="F133" s="2" t="s">
         <v>19</v>
@@ -5909,17 +5909,17 @@
       <c r="B134" s="2">
         <v>133</v>
       </c>
-      <c r="C134" s="5" t="s">
-        <v>11</v>
+      <c r="C134" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G134" s="3"/>
       <c r="H134" s="3"/>
@@ -5948,17 +5948,17 @@
       <c r="B135" s="2">
         <v>134</v>
       </c>
-      <c r="C135" s="5" t="s">
-        <v>11</v>
+      <c r="C135" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E135" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="F135" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G135" s="3"/>
       <c r="H135" s="3"/>
@@ -5988,16 +5988,16 @@
         <v>135</v>
       </c>
       <c r="C136" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="E136" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F136" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G136" s="3"/>
       <c r="H136" s="3"/>
@@ -6030,13 +6030,13 @@
         <v>11</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
       <c r="E137" s="2" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="F137" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G137" s="3"/>
       <c r="H137" s="3"/>
@@ -6069,13 +6069,13 @@
         <v>11</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="E138" s="2" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="F138" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G138" s="3"/>
       <c r="H138" s="3"/>
@@ -6105,16 +6105,16 @@
         <v>138</v>
       </c>
       <c r="C139" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E139" s="2" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="F139" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G139" s="3"/>
       <c r="H139" s="3"/>
@@ -6147,33 +6147,33 @@
         <v>11</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E140" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F140" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G140" s="2"/>
-      <c r="H140" s="2"/>
-      <c r="I140" s="2"/>
-      <c r="J140" s="2"/>
-      <c r="K140" s="2"/>
-      <c r="L140" s="2"/>
-      <c r="M140" s="2"/>
-      <c r="N140" s="2"/>
-      <c r="O140" s="2"/>
-      <c r="P140" s="2"/>
-      <c r="Q140" s="2"/>
-      <c r="R140" s="2"/>
-      <c r="S140" s="2"/>
-      <c r="T140" s="2"/>
-      <c r="U140" s="2"/>
-      <c r="V140" s="2"/>
-      <c r="W140" s="2"/>
-      <c r="X140" s="2"/>
-      <c r="Y140" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="G140" s="3"/>
+      <c r="H140" s="3"/>
+      <c r="I140" s="3"/>
+      <c r="J140" s="3"/>
+      <c r="K140" s="3"/>
+      <c r="L140" s="3"/>
+      <c r="M140" s="3"/>
+      <c r="N140" s="3"/>
+      <c r="O140" s="3"/>
+      <c r="P140" s="3"/>
+      <c r="Q140" s="3"/>
+      <c r="R140" s="3"/>
+      <c r="S140" s="3"/>
+      <c r="T140" s="3"/>
+      <c r="U140" s="3"/>
+      <c r="V140" s="3"/>
+      <c r="W140" s="3"/>
+      <c r="X140" s="3"/>
+      <c r="Y140" s="3"/>
     </row>
     <row r="141" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
@@ -6186,7 +6186,7 @@
         <v>11</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E141" s="2" t="s">
         <v>57</v>
@@ -6194,25 +6194,25 @@
       <c r="F141" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G141" s="2"/>
-      <c r="H141" s="2"/>
-      <c r="I141" s="2"/>
-      <c r="J141" s="2"/>
-      <c r="K141" s="2"/>
-      <c r="L141" s="2"/>
-      <c r="M141" s="2"/>
-      <c r="N141" s="2"/>
-      <c r="O141" s="2"/>
-      <c r="P141" s="2"/>
-      <c r="Q141" s="2"/>
-      <c r="R141" s="2"/>
-      <c r="S141" s="2"/>
-      <c r="T141" s="2"/>
-      <c r="U141" s="2"/>
-      <c r="V141" s="2"/>
-      <c r="W141" s="2"/>
-      <c r="X141" s="2"/>
-      <c r="Y141" s="2"/>
+      <c r="G141" s="3"/>
+      <c r="H141" s="3"/>
+      <c r="I141" s="3"/>
+      <c r="J141" s="3"/>
+      <c r="K141" s="3"/>
+      <c r="L141" s="3"/>
+      <c r="M141" s="3"/>
+      <c r="N141" s="3"/>
+      <c r="O141" s="3"/>
+      <c r="P141" s="3"/>
+      <c r="Q141" s="3"/>
+      <c r="R141" s="3"/>
+      <c r="S141" s="3"/>
+      <c r="T141" s="3"/>
+      <c r="U141" s="3"/>
+      <c r="V141" s="3"/>
+      <c r="W141" s="3"/>
+      <c r="X141" s="3"/>
+      <c r="Y141" s="3"/>
     </row>
     <row r="142" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
@@ -6225,7 +6225,7 @@
         <v>11</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E142" s="2" t="s">
         <v>57</v>
@@ -6233,25 +6233,25 @@
       <c r="F142" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G142" s="2"/>
-      <c r="H142" s="2"/>
-      <c r="I142" s="2"/>
-      <c r="J142" s="2"/>
-      <c r="K142" s="2"/>
-      <c r="L142" s="2"/>
-      <c r="M142" s="2"/>
-      <c r="N142" s="2"/>
-      <c r="O142" s="2"/>
-      <c r="P142" s="2"/>
-      <c r="Q142" s="2"/>
-      <c r="R142" s="2"/>
-      <c r="S142" s="2"/>
-      <c r="T142" s="2"/>
-      <c r="U142" s="2"/>
-      <c r="V142" s="2"/>
-      <c r="W142" s="2"/>
-      <c r="X142" s="2"/>
-      <c r="Y142" s="2"/>
+      <c r="G142" s="3"/>
+      <c r="H142" s="3"/>
+      <c r="I142" s="3"/>
+      <c r="J142" s="3"/>
+      <c r="K142" s="3"/>
+      <c r="L142" s="3"/>
+      <c r="M142" s="3"/>
+      <c r="N142" s="3"/>
+      <c r="O142" s="3"/>
+      <c r="P142" s="3"/>
+      <c r="Q142" s="3"/>
+      <c r="R142" s="3"/>
+      <c r="S142" s="3"/>
+      <c r="T142" s="3"/>
+      <c r="U142" s="3"/>
+      <c r="V142" s="3"/>
+      <c r="W142" s="3"/>
+      <c r="X142" s="3"/>
+      <c r="Y142" s="3"/>
     </row>
     <row r="143" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
@@ -6264,7 +6264,7 @@
         <v>11</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E143" s="2" t="s">
         <v>57</v>
@@ -6303,7 +6303,7 @@
         <v>11</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="E144" s="2" t="s">
         <v>57</v>
@@ -6342,13 +6342,13 @@
         <v>11</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E145" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F145" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G145" s="2"/>
       <c r="H145" s="2"/>
@@ -6377,17 +6377,17 @@
       <c r="B146" s="2">
         <v>145</v>
       </c>
-      <c r="C146" s="2" t="s">
-        <v>7</v>
+      <c r="C146" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E146" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F146" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G146" s="2"/>
       <c r="H146" s="2"/>
@@ -6417,16 +6417,16 @@
         <v>146</v>
       </c>
       <c r="C147" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D147" s="10" t="s">
-        <v>89</v>
+        <v>11</v>
+      </c>
+      <c r="D147" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="E147" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F147" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G147" s="2"/>
       <c r="H147" s="2"/>
@@ -6456,16 +6456,16 @@
         <v>147</v>
       </c>
       <c r="C148" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E148" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F148" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G148" s="2"/>
       <c r="H148" s="2"/>
@@ -6497,14 +6497,14 @@
       <c r="C149" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D149" s="10" t="s">
-        <v>67</v>
+      <c r="D149" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="E149" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F149" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G149" s="2"/>
       <c r="H149" s="2"/>
@@ -6536,8 +6536,8 @@
       <c r="C150" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D150" s="3" t="s">
-        <v>68</v>
+      <c r="D150" s="10" t="s">
+        <v>89</v>
       </c>
       <c r="E150" s="2" t="s">
         <v>9</v>
@@ -6576,7 +6576,7 @@
         <v>7</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E151" s="2" t="s">
         <v>9</v>
@@ -6611,17 +6611,17 @@
       <c r="B152" s="2">
         <v>151</v>
       </c>
-      <c r="C152" s="5" t="s">
-        <v>11</v>
+      <c r="C152" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D152" s="10" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="E152" s="2" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="F152" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G152" s="2"/>
       <c r="H152" s="2"/>
@@ -6644,12 +6644,24 @@
       <c r="Y152" s="2"/>
     </row>
     <row r="153" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A153" s="2"/>
-      <c r="B153" s="2"/>
-      <c r="C153" s="5"/>
-      <c r="D153" s="3"/>
-      <c r="E153" s="2"/>
-      <c r="F153" s="2"/>
+      <c r="A153" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B153" s="2">
+        <v>152</v>
+      </c>
+      <c r="C153" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D153" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E153" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F153" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="G153" s="2"/>
       <c r="H153" s="2"/>
       <c r="I153" s="2"/>
@@ -6671,12 +6683,24 @@
       <c r="Y153" s="2"/>
     </row>
     <row r="154" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A154" s="2"/>
-      <c r="B154" s="2"/>
-      <c r="C154" s="5"/>
-      <c r="D154" s="3"/>
-      <c r="E154" s="2"/>
-      <c r="F154" s="2"/>
+      <c r="A154" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B154" s="2">
+        <v>153</v>
+      </c>
+      <c r="C154" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D154" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E154" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F154" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="G154" s="2"/>
       <c r="H154" s="2"/>
       <c r="I154" s="2"/>
@@ -6698,12 +6722,24 @@
       <c r="Y154" s="2"/>
     </row>
     <row r="155" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A155" s="2"/>
-      <c r="B155" s="2"/>
-      <c r="C155" s="5"/>
-      <c r="D155" s="3"/>
-      <c r="E155" s="2"/>
-      <c r="F155" s="2"/>
+      <c r="A155" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B155" s="2">
+        <v>154</v>
+      </c>
+      <c r="C155" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D155" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E155" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F155" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="G155" s="2"/>
       <c r="H155" s="2"/>
       <c r="I155" s="2"/>
@@ -6781,7 +6817,7 @@
     <row r="158" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A158" s="2"/>
       <c r="B158" s="2"/>
-      <c r="C158" s="2"/>
+      <c r="C158" s="5"/>
       <c r="D158" s="3"/>
       <c r="E158" s="2"/>
       <c r="F158" s="2"/>
@@ -6862,7 +6898,7 @@
     <row r="161" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A161" s="2"/>
       <c r="B161" s="2"/>
-      <c r="C161" s="5"/>
+      <c r="C161" s="2"/>
       <c r="D161" s="3"/>
       <c r="E161" s="2"/>
       <c r="F161" s="2"/>
@@ -6916,8 +6952,8 @@
     <row r="163" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A163" s="2"/>
       <c r="B163" s="2"/>
-      <c r="C163" s="2"/>
-      <c r="D163" s="2"/>
+      <c r="C163" s="5"/>
+      <c r="D163" s="3"/>
       <c r="E163" s="2"/>
       <c r="F163" s="2"/>
       <c r="G163" s="2"/>
@@ -6943,8 +6979,8 @@
     <row r="164" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A164" s="2"/>
       <c r="B164" s="2"/>
-      <c r="C164" s="2"/>
-      <c r="D164" s="2"/>
+      <c r="C164" s="5"/>
+      <c r="D164" s="3"/>
       <c r="E164" s="2"/>
       <c r="F164" s="2"/>
       <c r="G164" s="2"/>
@@ -6970,8 +7006,8 @@
     <row r="165" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A165" s="2"/>
       <c r="B165" s="2"/>
-      <c r="C165" s="2"/>
-      <c r="D165" s="2"/>
+      <c r="C165" s="5"/>
+      <c r="D165" s="3"/>
       <c r="E165" s="2"/>
       <c r="F165" s="2"/>
       <c r="G165" s="2"/>
@@ -28405,6 +28441,87 @@
       <c r="X958" s="2"/>
       <c r="Y958" s="2"/>
     </row>
+    <row r="959" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A959" s="2"/>
+      <c r="B959" s="2"/>
+      <c r="C959" s="2"/>
+      <c r="D959" s="2"/>
+      <c r="E959" s="2"/>
+      <c r="F959" s="2"/>
+      <c r="G959" s="2"/>
+      <c r="H959" s="2"/>
+      <c r="I959" s="2"/>
+      <c r="J959" s="2"/>
+      <c r="K959" s="2"/>
+      <c r="L959" s="2"/>
+      <c r="M959" s="2"/>
+      <c r="N959" s="2"/>
+      <c r="O959" s="2"/>
+      <c r="P959" s="2"/>
+      <c r="Q959" s="2"/>
+      <c r="R959" s="2"/>
+      <c r="S959" s="2"/>
+      <c r="T959" s="2"/>
+      <c r="U959" s="2"/>
+      <c r="V959" s="2"/>
+      <c r="W959" s="2"/>
+      <c r="X959" s="2"/>
+      <c r="Y959" s="2"/>
+    </row>
+    <row r="960" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A960" s="2"/>
+      <c r="B960" s="2"/>
+      <c r="C960" s="2"/>
+      <c r="D960" s="2"/>
+      <c r="E960" s="2"/>
+      <c r="F960" s="2"/>
+      <c r="G960" s="2"/>
+      <c r="H960" s="2"/>
+      <c r="I960" s="2"/>
+      <c r="J960" s="2"/>
+      <c r="K960" s="2"/>
+      <c r="L960" s="2"/>
+      <c r="M960" s="2"/>
+      <c r="N960" s="2"/>
+      <c r="O960" s="2"/>
+      <c r="P960" s="2"/>
+      <c r="Q960" s="2"/>
+      <c r="R960" s="2"/>
+      <c r="S960" s="2"/>
+      <c r="T960" s="2"/>
+      <c r="U960" s="2"/>
+      <c r="V960" s="2"/>
+      <c r="W960" s="2"/>
+      <c r="X960" s="2"/>
+      <c r="Y960" s="2"/>
+    </row>
+    <row r="961" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A961" s="2"/>
+      <c r="B961" s="2"/>
+      <c r="C961" s="2"/>
+      <c r="D961" s="2"/>
+      <c r="E961" s="2"/>
+      <c r="F961" s="2"/>
+      <c r="G961" s="2"/>
+      <c r="H961" s="2"/>
+      <c r="I961" s="2"/>
+      <c r="J961" s="2"/>
+      <c r="K961" s="2"/>
+      <c r="L961" s="2"/>
+      <c r="M961" s="2"/>
+      <c r="N961" s="2"/>
+      <c r="O961" s="2"/>
+      <c r="P961" s="2"/>
+      <c r="Q961" s="2"/>
+      <c r="R961" s="2"/>
+      <c r="S961" s="2"/>
+      <c r="T961" s="2"/>
+      <c r="U961" s="2"/>
+      <c r="V961" s="2"/>
+      <c r="W961" s="2"/>
+      <c r="X961" s="2"/>
+      <c r="Y961" s="2"/>
+    </row>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{49968090-594F-4035-ABCC-088176AC5527}" filter="1" showAutoFilter="1">
@@ -28412,7 +28529,7 @@
       <autoFilter ref="A1:A950"/>
     </customSheetView>
   </customSheetViews>
-  <conditionalFormatting sqref="G1 F1:F958">
+  <conditionalFormatting sqref="G1 F1:F961">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Read">
       <formula>NOT(ISERROR(SEARCH(("Read"),(F1))))</formula>
     </cfRule>

</xml_diff>

<commit_message>
Updated permissions for Intake Form for ALSP user.
</commit_message>
<xml_diff>
--- a/Roles and Permissions.xlsx
+++ b/Roles and Permissions.xlsx
@@ -16,7 +16,7 @@
     <sheet name="ScreenIds" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Z_49968090_594F_4035_ABCC_088176AC5527_.wvu.FilterData" localSheetId="0" hidden="1">'Roles and Permissions'!$A$1:$A$963</definedName>
+    <definedName name="Z_49968090_594F_4035_ABCC_088176AC5527_.wvu.FilterData" localSheetId="0" hidden="1">'Roles and Permissions'!$A$1:$A$964</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <customWorkbookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="91">
   <si>
     <t>User</t>
   </si>
@@ -700,10 +700,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Y963"/>
+  <dimension ref="A1:Y964"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A147" workbookViewId="0">
-      <selection activeCell="B161" sqref="B161"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2360,17 +2360,17 @@
       <c r="B43" s="2">
         <v>42</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>22</v>
+        <v>79</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
@@ -2403,7 +2403,7 @@
         <v>11</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>17</v>
@@ -2438,11 +2438,11 @@
       <c r="B45" s="2">
         <v>44</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>17</v>
@@ -2472,22 +2472,22 @@
     </row>
     <row r="46" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B46" s="2">
         <v>45</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
@@ -2517,13 +2517,13 @@
         <v>46</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>10</v>
@@ -2559,10 +2559,10 @@
         <v>11</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E48" s="15" t="s">
         <v>13</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>10</v>
@@ -2597,8 +2597,8 @@
       <c r="C49" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D49" s="10" t="s">
-        <v>14</v>
+      <c r="D49" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="E49" s="15" t="s">
         <v>13</v>
@@ -2627,7 +2627,7 @@
       <c r="Y49" s="2"/>
     </row>
     <row r="50" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A50" s="15" t="s">
+      <c r="A50" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B50" s="2">
@@ -2637,10 +2637,10 @@
         <v>11</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>78</v>
+        <v>14</v>
       </c>
       <c r="E50" s="15" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>10</v>
@@ -2666,7 +2666,7 @@
       <c r="Y50" s="2"/>
     </row>
     <row r="51" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="15" t="s">
         <v>44</v>
       </c>
       <c r="B51" s="2">
@@ -2675,8 +2675,8 @@
       <c r="C51" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D51" s="3" t="s">
-        <v>15</v>
+      <c r="D51" s="10" t="s">
+        <v>78</v>
       </c>
       <c r="E51" s="15" t="s">
         <v>8</v>
@@ -2715,9 +2715,9 @@
         <v>11</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E52" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E52" s="15" t="s">
         <v>8</v>
       </c>
       <c r="F52" s="2" t="s">
@@ -2751,16 +2751,16 @@
         <v>52</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
@@ -2790,13 +2790,13 @@
         <v>53</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>19</v>
@@ -2832,7 +2832,7 @@
         <v>11</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>88</v>
+        <v>18</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>17</v>
@@ -2871,7 +2871,7 @@
         <v>11</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>20</v>
+        <v>88</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>17</v>
@@ -2910,7 +2910,7 @@
         <v>11</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>17</v>
@@ -2949,7 +2949,7 @@
         <v>11</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>17</v>
@@ -2988,7 +2988,7 @@
         <v>11</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>17</v>
@@ -3027,7 +3027,7 @@
         <v>11</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>17</v>
@@ -3063,16 +3063,16 @@
         <v>60</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
@@ -3105,7 +3105,7 @@
         <v>7</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>9</v>
@@ -3141,16 +3141,16 @@
         <v>62</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
@@ -3179,11 +3179,11 @@
       <c r="B64" s="2">
         <v>63</v>
       </c>
-      <c r="C64" s="5" t="s">
+      <c r="C64" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>26</v>
@@ -3222,7 +3222,7 @@
         <v>11</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>26</v>
@@ -3257,17 +3257,17 @@
       <c r="B66" s="2">
         <v>65</v>
       </c>
-      <c r="C66" s="2" t="s">
-        <v>7</v>
+      <c r="C66" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
@@ -3299,11 +3299,11 @@
       <c r="C67" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D67" s="10" t="s">
-        <v>90</v>
+      <c r="D67" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>10</v>
@@ -3336,13 +3336,13 @@
         <v>67</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>31</v>
+        <v>7</v>
+      </c>
+      <c r="D68" s="10" t="s">
+        <v>90</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>90</v>
+        <v>9</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>10</v>
@@ -3378,10 +3378,10 @@
         <v>11</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>10</v>
@@ -3417,13 +3417,13 @@
         <v>11</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
@@ -3456,13 +3456,13 @@
         <v>11</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
@@ -3492,16 +3492,16 @@
         <v>71</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
@@ -3530,14 +3530,14 @@
       <c r="B73" s="2">
         <v>72</v>
       </c>
-      <c r="C73" s="5" t="s">
-        <v>11</v>
+      <c r="C73" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="F73" s="2" t="s">
         <v>19</v>
@@ -3573,7 +3573,7 @@
         <v>11</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>45</v>
@@ -3612,7 +3612,7 @@
         <v>11</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>45</v>
@@ -3648,13 +3648,13 @@
         <v>75</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="F76" s="2" t="s">
         <v>19</v>
@@ -3687,16 +3687,16 @@
         <v>76</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
@@ -3729,10 +3729,10 @@
         <v>11</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="F78" s="2" t="s">
         <v>10</v>
@@ -3768,13 +3768,13 @@
         <v>11</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>35</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
@@ -3807,13 +3807,13 @@
         <v>11</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>35</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
@@ -3846,10 +3846,10 @@
         <v>11</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>79</v>
+        <v>36</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F81" s="2" t="s">
         <v>10</v>
@@ -3876,19 +3876,19 @@
     </row>
     <row r="82" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B82" s="2">
         <v>81</v>
       </c>
-      <c r="C82" s="2" t="s">
-        <v>7</v>
+      <c r="C82" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>50</v>
+        <v>79</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="F82" s="2" t="s">
         <v>10</v>
@@ -3924,13 +3924,13 @@
         <v>7</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
@@ -3960,13 +3960,13 @@
         <v>83</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F84" s="2" t="s">
         <v>19</v>
@@ -4002,7 +4002,7 @@
         <v>11</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>88</v>
+        <v>18</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>17</v>
@@ -4041,7 +4041,7 @@
         <v>11</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>20</v>
+        <v>88</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>17</v>
@@ -4080,7 +4080,7 @@
         <v>11</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>17</v>
@@ -4119,7 +4119,7 @@
         <v>11</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>17</v>
@@ -4158,7 +4158,7 @@
         <v>11</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>17</v>
@@ -4197,7 +4197,7 @@
         <v>11</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>17</v>
@@ -4233,13 +4233,13 @@
         <v>90</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F91" s="2" t="s">
         <v>19</v>
@@ -4272,13 +4272,13 @@
         <v>91</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="F92" s="2" t="s">
         <v>19</v>
@@ -4314,7 +4314,7 @@
         <v>11</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>51</v>
@@ -4353,7 +4353,7 @@
         <v>11</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>51</v>
@@ -4388,11 +4388,11 @@
       <c r="B95" s="2">
         <v>94</v>
       </c>
-      <c r="C95" s="5" t="s">
+      <c r="C95" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>51</v>
@@ -4431,7 +4431,7 @@
         <v>11</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>51</v>
@@ -4466,17 +4466,17 @@
       <c r="B97" s="2">
         <v>96</v>
       </c>
-      <c r="C97" s="2" t="s">
-        <v>7</v>
+      <c r="C97" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
@@ -4509,7 +4509,7 @@
         <v>7</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>9</v>
@@ -4544,17 +4544,17 @@
       <c r="B99" s="2">
         <v>98</v>
       </c>
-      <c r="C99" s="5" t="s">
-        <v>11</v>
+      <c r="C99" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
@@ -4587,7 +4587,7 @@
         <v>11</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>26</v>
@@ -4626,7 +4626,7 @@
         <v>11</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>26</v>
@@ -4662,16 +4662,16 @@
         <v>101</v>
       </c>
       <c r="C102" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G102" s="2"/>
       <c r="H102" s="2"/>
@@ -4701,13 +4701,13 @@
         <v>102</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="F103" s="2" t="s">
         <v>10</v>
@@ -4743,7 +4743,7 @@
         <v>11</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E104" s="2" t="s">
         <v>57</v>
@@ -4782,13 +4782,13 @@
         <v>11</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G105" s="2"/>
       <c r="H105" s="2"/>
@@ -4821,7 +4821,7 @@
         <v>11</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>57</v>
@@ -4860,13 +4860,13 @@
         <v>11</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G107" s="2"/>
       <c r="H107" s="2"/>
@@ -4899,13 +4899,13 @@
         <v>11</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G108" s="2"/>
       <c r="H108" s="2"/>
@@ -4938,7 +4938,7 @@
         <v>11</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>57</v>
@@ -4977,13 +4977,13 @@
         <v>11</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G110" s="2"/>
       <c r="H110" s="2"/>
@@ -5016,7 +5016,7 @@
         <v>11</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>57</v>
@@ -5044,83 +5044,83 @@
       <c r="X111" s="2"/>
       <c r="Y111" s="2"/>
     </row>
-    <row r="112" spans="1:25" s="18" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A112" s="13" t="s">
+    <row r="112" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B112" s="2">
         <v>111</v>
       </c>
-      <c r="C112" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D112" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="E112" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F112" s="13" t="s">
+      <c r="C112" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D112" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F112" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G112" s="13"/>
-      <c r="H112" s="13"/>
-      <c r="I112" s="13"/>
-      <c r="J112" s="13"/>
-      <c r="K112" s="13"/>
-      <c r="L112" s="13"/>
-      <c r="M112" s="13"/>
-      <c r="N112" s="13"/>
-      <c r="O112" s="13"/>
-      <c r="P112" s="13"/>
-      <c r="Q112" s="13"/>
-      <c r="R112" s="13"/>
-      <c r="S112" s="13"/>
-      <c r="T112" s="13"/>
-      <c r="U112" s="13"/>
-      <c r="V112" s="13"/>
-      <c r="W112" s="13"/>
-      <c r="X112" s="13"/>
-      <c r="Y112" s="13"/>
-    </row>
-    <row r="113" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A113" s="2" t="s">
+      <c r="G112" s="2"/>
+      <c r="H112" s="2"/>
+      <c r="I112" s="2"/>
+      <c r="J112" s="2"/>
+      <c r="K112" s="2"/>
+      <c r="L112" s="2"/>
+      <c r="M112" s="2"/>
+      <c r="N112" s="2"/>
+      <c r="O112" s="2"/>
+      <c r="P112" s="2"/>
+      <c r="Q112" s="2"/>
+      <c r="R112" s="2"/>
+      <c r="S112" s="2"/>
+      <c r="T112" s="2"/>
+      <c r="U112" s="2"/>
+      <c r="V112" s="2"/>
+      <c r="W112" s="2"/>
+      <c r="X112" s="2"/>
+      <c r="Y112" s="2"/>
+    </row>
+    <row r="113" spans="1:25" s="18" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A113" s="13" t="s">
         <v>49</v>
       </c>
       <c r="B113" s="2">
         <v>112</v>
       </c>
-      <c r="C113" s="5" t="s">
+      <c r="C113" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D113" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E113" s="2" t="s">
+      <c r="D113" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E113" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F113" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G113" s="2"/>
-      <c r="H113" s="2"/>
-      <c r="I113" s="2"/>
-      <c r="J113" s="2"/>
-      <c r="K113" s="2"/>
-      <c r="L113" s="2"/>
-      <c r="M113" s="2"/>
-      <c r="N113" s="2"/>
-      <c r="O113" s="2"/>
-      <c r="P113" s="2"/>
-      <c r="Q113" s="2"/>
-      <c r="R113" s="2"/>
-      <c r="S113" s="2"/>
-      <c r="T113" s="2"/>
-      <c r="U113" s="2"/>
-      <c r="V113" s="2"/>
-      <c r="W113" s="2"/>
-      <c r="X113" s="2"/>
-      <c r="Y113" s="2"/>
+      <c r="F113" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G113" s="13"/>
+      <c r="H113" s="13"/>
+      <c r="I113" s="13"/>
+      <c r="J113" s="13"/>
+      <c r="K113" s="13"/>
+      <c r="L113" s="13"/>
+      <c r="M113" s="13"/>
+      <c r="N113" s="13"/>
+      <c r="O113" s="13"/>
+      <c r="P113" s="13"/>
+      <c r="Q113" s="13"/>
+      <c r="R113" s="13"/>
+      <c r="S113" s="13"/>
+      <c r="T113" s="13"/>
+      <c r="U113" s="13"/>
+      <c r="V113" s="13"/>
+      <c r="W113" s="13"/>
+      <c r="X113" s="13"/>
+      <c r="Y113" s="13"/>
     </row>
     <row r="114" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
@@ -5133,7 +5133,7 @@
         <v>7</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>9</v>
@@ -5172,7 +5172,7 @@
         <v>7</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E115" s="2" t="s">
         <v>9</v>
@@ -5211,7 +5211,7 @@
         <v>7</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E116" s="2" t="s">
         <v>9</v>
@@ -5250,7 +5250,7 @@
         <v>7</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>9</v>
@@ -5279,43 +5279,43 @@
       <c r="Y117" s="2"/>
     </row>
     <row r="118" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A118" s="3" t="s">
+      <c r="A118" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B118" s="2">
         <v>117</v>
       </c>
-      <c r="C118" s="3" t="s">
+      <c r="C118" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D118" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="E118" s="3" t="s">
+      <c r="D118" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E118" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F118" s="6" t="s">
+      <c r="F118" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G118" s="3"/>
-      <c r="H118" s="3"/>
-      <c r="I118" s="3"/>
-      <c r="J118" s="3"/>
-      <c r="K118" s="3"/>
-      <c r="L118" s="3"/>
-      <c r="M118" s="3"/>
-      <c r="N118" s="3"/>
-      <c r="O118" s="3"/>
-      <c r="P118" s="3"/>
-      <c r="Q118" s="3"/>
-      <c r="R118" s="3"/>
-      <c r="S118" s="3"/>
-      <c r="T118" s="3"/>
-      <c r="U118" s="3"/>
-      <c r="V118" s="3"/>
-      <c r="W118" s="3"/>
-      <c r="X118" s="3"/>
-      <c r="Y118" s="3"/>
+      <c r="G118" s="2"/>
+      <c r="H118" s="2"/>
+      <c r="I118" s="2"/>
+      <c r="J118" s="2"/>
+      <c r="K118" s="2"/>
+      <c r="L118" s="2"/>
+      <c r="M118" s="2"/>
+      <c r="N118" s="2"/>
+      <c r="O118" s="2"/>
+      <c r="P118" s="2"/>
+      <c r="Q118" s="2"/>
+      <c r="R118" s="2"/>
+      <c r="S118" s="2"/>
+      <c r="T118" s="2"/>
+      <c r="U118" s="2"/>
+      <c r="V118" s="2"/>
+      <c r="W118" s="2"/>
+      <c r="X118" s="2"/>
+      <c r="Y118" s="2"/>
     </row>
     <row r="119" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
@@ -5328,7 +5328,7 @@
         <v>7</v>
       </c>
       <c r="D119" s="10" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="E119" s="3" t="s">
         <v>9</v>
@@ -5364,13 +5364,13 @@
         <v>119</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D120" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E120" s="10" t="s">
         <v>90</v>
+      </c>
+      <c r="E120" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="F120" s="6" t="s">
         <v>19</v>
@@ -5396,23 +5396,23 @@
       <c r="Y120" s="3"/>
     </row>
     <row r="121" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A121" s="2" t="s">
-        <v>70</v>
+      <c r="A121" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="B121" s="2">
         <v>120</v>
       </c>
-      <c r="C121" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D121" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E121" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F121" s="2" t="s">
-        <v>10</v>
+      <c r="C121" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D121" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E121" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="F121" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="G121" s="3"/>
       <c r="H121" s="3"/>
@@ -5445,13 +5445,13 @@
         <v>7</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="E122" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G122" s="3"/>
       <c r="H122" s="3"/>
@@ -5481,13 +5481,13 @@
         <v>122</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E123" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F123" s="2" t="s">
         <v>19</v>
@@ -5522,8 +5522,8 @@
       <c r="C124" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D124" s="10" t="s">
-        <v>88</v>
+      <c r="D124" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="E124" s="2" t="s">
         <v>17</v>
@@ -5561,8 +5561,8 @@
       <c r="C125" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D125" s="3" t="s">
-        <v>20</v>
+      <c r="D125" s="10" t="s">
+        <v>88</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>17</v>
@@ -5601,7 +5601,7 @@
         <v>11</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>17</v>
@@ -5640,7 +5640,7 @@
         <v>11</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E127" s="2" t="s">
         <v>17</v>
@@ -5679,7 +5679,7 @@
         <v>11</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E128" s="2" t="s">
         <v>17</v>
@@ -5718,7 +5718,7 @@
         <v>11</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E129" s="2" t="s">
         <v>17</v>
@@ -5754,13 +5754,13 @@
         <v>129</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="E130" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F130" s="2" t="s">
         <v>19</v>
@@ -5793,13 +5793,13 @@
         <v>130</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E131" s="2" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="F131" s="2" t="s">
         <v>19</v>
@@ -5835,7 +5835,7 @@
         <v>11</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>51</v>
@@ -5874,7 +5874,7 @@
         <v>11</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E133" s="2" t="s">
         <v>51</v>
@@ -5909,11 +5909,11 @@
       <c r="B134" s="2">
         <v>133</v>
       </c>
-      <c r="C134" s="5" t="s">
+      <c r="C134" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E134" s="2" t="s">
         <v>51</v>
@@ -5952,7 +5952,7 @@
         <v>11</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E135" s="2" t="s">
         <v>51</v>
@@ -5987,17 +5987,17 @@
       <c r="B136" s="2">
         <v>135</v>
       </c>
-      <c r="C136" s="2" t="s">
-        <v>7</v>
+      <c r="C136" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="E136" s="2" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="F136" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G136" s="3"/>
       <c r="H136" s="3"/>
@@ -6030,7 +6030,7 @@
         <v>7</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E137" s="2" t="s">
         <v>9</v>
@@ -6065,17 +6065,17 @@
       <c r="B138" s="2">
         <v>137</v>
       </c>
-      <c r="C138" s="5" t="s">
-        <v>11</v>
+      <c r="C138" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E138" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="F138" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G138" s="3"/>
       <c r="H138" s="3"/>
@@ -6108,7 +6108,7 @@
         <v>11</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E139" s="2" t="s">
         <v>26</v>
@@ -6147,7 +6147,7 @@
         <v>11</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E140" s="2" t="s">
         <v>26</v>
@@ -6183,16 +6183,16 @@
         <v>140</v>
       </c>
       <c r="C141" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="E141" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F141" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G141" s="3"/>
       <c r="H141" s="3"/>
@@ -6222,13 +6222,13 @@
         <v>141</v>
       </c>
       <c r="C142" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E142" s="2" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="F142" s="2" t="s">
         <v>10</v>
@@ -6264,7 +6264,7 @@
         <v>11</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E143" s="2" t="s">
         <v>57</v>
@@ -6303,13 +6303,13 @@
         <v>11</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E144" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F144" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G144" s="3"/>
       <c r="H144" s="3"/>
@@ -6342,7 +6342,7 @@
         <v>11</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E145" s="2" t="s">
         <v>57</v>
@@ -6350,25 +6350,25 @@
       <c r="F145" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G145" s="2"/>
-      <c r="H145" s="2"/>
-      <c r="I145" s="2"/>
-      <c r="J145" s="2"/>
-      <c r="K145" s="2"/>
-      <c r="L145" s="2"/>
-      <c r="M145" s="2"/>
-      <c r="N145" s="2"/>
-      <c r="O145" s="2"/>
-      <c r="P145" s="2"/>
-      <c r="Q145" s="2"/>
-      <c r="R145" s="2"/>
-      <c r="S145" s="2"/>
-      <c r="T145" s="2"/>
-      <c r="U145" s="2"/>
-      <c r="V145" s="2"/>
-      <c r="W145" s="2"/>
-      <c r="X145" s="2"/>
-      <c r="Y145" s="2"/>
+      <c r="G145" s="3"/>
+      <c r="H145" s="3"/>
+      <c r="I145" s="3"/>
+      <c r="J145" s="3"/>
+      <c r="K145" s="3"/>
+      <c r="L145" s="3"/>
+      <c r="M145" s="3"/>
+      <c r="N145" s="3"/>
+      <c r="O145" s="3"/>
+      <c r="P145" s="3"/>
+      <c r="Q145" s="3"/>
+      <c r="R145" s="3"/>
+      <c r="S145" s="3"/>
+      <c r="T145" s="3"/>
+      <c r="U145" s="3"/>
+      <c r="V145" s="3"/>
+      <c r="W145" s="3"/>
+      <c r="X145" s="3"/>
+      <c r="Y145" s="3"/>
     </row>
     <row r="146" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
@@ -6381,13 +6381,13 @@
         <v>11</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E146" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F146" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G146" s="2"/>
       <c r="H146" s="2"/>
@@ -6420,13 +6420,13 @@
         <v>11</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E147" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F147" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G147" s="2"/>
       <c r="H147" s="2"/>
@@ -6459,7 +6459,7 @@
         <v>11</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E148" s="2" t="s">
         <v>57</v>
@@ -6498,13 +6498,13 @@
         <v>11</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="E149" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F149" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G149" s="2"/>
       <c r="H149" s="2"/>
@@ -6537,7 +6537,7 @@
         <v>11</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="E150" s="2" t="s">
         <v>57</v>
@@ -6572,14 +6572,14 @@
       <c r="B151" s="2">
         <v>150</v>
       </c>
-      <c r="C151" s="2" t="s">
-        <v>7</v>
+      <c r="C151" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E151" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F151" s="2" t="s">
         <v>10</v>
@@ -6611,17 +6611,17 @@
       <c r="B152" s="2">
         <v>151</v>
       </c>
-      <c r="C152" s="5" t="s">
+      <c r="C152" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D152" s="10" t="s">
-        <v>89</v>
+      <c r="D152" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="E152" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F152" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G152" s="2"/>
       <c r="H152" s="2"/>
@@ -6653,8 +6653,8 @@
       <c r="C153" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D153" s="3" t="s">
-        <v>71</v>
+      <c r="D153" s="10" t="s">
+        <v>89</v>
       </c>
       <c r="E153" s="2" t="s">
         <v>9</v>
@@ -6689,11 +6689,11 @@
       <c r="B154" s="2">
         <v>153</v>
       </c>
-      <c r="C154" s="2" t="s">
+      <c r="C154" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D154" s="10" t="s">
-        <v>67</v>
+      <c r="D154" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="E154" s="2" t="s">
         <v>9</v>
@@ -6728,11 +6728,11 @@
       <c r="B155" s="2">
         <v>154</v>
       </c>
-      <c r="C155" s="5" t="s">
+      <c r="C155" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D155" s="3" t="s">
-        <v>68</v>
+      <c r="D155" s="10" t="s">
+        <v>67</v>
       </c>
       <c r="E155" s="2" t="s">
         <v>9</v>
@@ -6771,7 +6771,7 @@
         <v>7</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E156" s="2" t="s">
         <v>9</v>
@@ -6807,16 +6807,16 @@
         <v>156</v>
       </c>
       <c r="C157" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D157" s="10" t="s">
-        <v>87</v>
+        <v>7</v>
+      </c>
+      <c r="D157" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="E157" s="2" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="F157" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G157" s="2"/>
       <c r="H157" s="2"/>
@@ -6839,12 +6839,24 @@
       <c r="Y157" s="2"/>
     </row>
     <row r="158" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A158" s="2"/>
-      <c r="B158" s="2"/>
-      <c r="C158" s="5"/>
-      <c r="D158" s="3"/>
-      <c r="E158" s="2"/>
-      <c r="F158" s="2"/>
+      <c r="A158" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B158" s="2">
+        <v>157</v>
+      </c>
+      <c r="C158" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D158" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E158" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F158" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="G158" s="2"/>
       <c r="H158" s="2"/>
       <c r="I158" s="2"/>
@@ -6976,7 +6988,7 @@
     <row r="163" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A163" s="2"/>
       <c r="B163" s="2"/>
-      <c r="C163" s="2"/>
+      <c r="C163" s="5"/>
       <c r="D163" s="3"/>
       <c r="E163" s="2"/>
       <c r="F163" s="2"/>
@@ -7003,7 +7015,7 @@
     <row r="164" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A164" s="2"/>
       <c r="B164" s="2"/>
-      <c r="C164" s="5"/>
+      <c r="C164" s="2"/>
       <c r="D164" s="3"/>
       <c r="E164" s="2"/>
       <c r="F164" s="2"/>
@@ -7111,8 +7123,8 @@
     <row r="168" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A168" s="2"/>
       <c r="B168" s="2"/>
-      <c r="C168" s="2"/>
-      <c r="D168" s="2"/>
+      <c r="C168" s="5"/>
+      <c r="D168" s="3"/>
       <c r="E168" s="2"/>
       <c r="F168" s="2"/>
       <c r="G168" s="2"/>
@@ -28600,6 +28612,33 @@
       <c r="X963" s="2"/>
       <c r="Y963" s="2"/>
     </row>
+    <row r="964" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A964" s="2"/>
+      <c r="B964" s="2"/>
+      <c r="C964" s="2"/>
+      <c r="D964" s="2"/>
+      <c r="E964" s="2"/>
+      <c r="F964" s="2"/>
+      <c r="G964" s="2"/>
+      <c r="H964" s="2"/>
+      <c r="I964" s="2"/>
+      <c r="J964" s="2"/>
+      <c r="K964" s="2"/>
+      <c r="L964" s="2"/>
+      <c r="M964" s="2"/>
+      <c r="N964" s="2"/>
+      <c r="O964" s="2"/>
+      <c r="P964" s="2"/>
+      <c r="Q964" s="2"/>
+      <c r="R964" s="2"/>
+      <c r="S964" s="2"/>
+      <c r="T964" s="2"/>
+      <c r="U964" s="2"/>
+      <c r="V964" s="2"/>
+      <c r="W964" s="2"/>
+      <c r="X964" s="2"/>
+      <c r="Y964" s="2"/>
+    </row>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{49968090-594F-4035-ABCC-088176AC5527}" filter="1" showAutoFilter="1">
@@ -28607,7 +28646,7 @@
       <autoFilter ref="A1:A950"/>
     </customSheetView>
   </customSheetViews>
-  <conditionalFormatting sqref="G1 F1:F963">
+  <conditionalFormatting sqref="G1 F1:F964">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Read">
       <formula>NOT(ISERROR(SEARCH(("Read"),(F1))))</formula>
     </cfRule>

</xml_diff>